<commit_message>
chore(Mapping Routes): Updating Functionnal Routes
Updating operationnal routes within adonisjs displayed through .edge files
</commit_message>
<xml_diff>
--- a/Docs/Routes Mapping.xlsx
+++ b/Docs/Routes Mapping.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv00wyv\Desktop\P_Bulle_Dev_FlashCards\latest\P_Bulle_Dev-Flashcards\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Full Stack Dev\Desktop\Trimestre 2\Projets\P_bulle\P_Bulle_Dev-Flashcards\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE800B2-5492-455D-9ABE-9242402CE623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC7E4E-E12C-4217-84E0-EA3119EBFAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78FF3FEE-8393-407A-AC41-6BC005ADEBC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{78FF3FEE-8393-407A-AC41-6BC005ADEBC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
   <si>
     <t>GET</t>
   </si>
@@ -188,9 +177,6 @@
     <t>Pour tous les utilisateurs</t>
   </si>
   <si>
-    <t>/decks/:deckId/cards</t>
-  </si>
-  <si>
     <t>Lister toutes les flashcards d’un deck</t>
   </si>
   <si>
@@ -248,14 +234,64 @@
     <t>Score, stats, option rejouer</t>
   </si>
   <si>
-    <t>/decks/:deckId/cards/:cardId</t>
+    <t>/decks/:deckId/flashcards</t>
+  </si>
+  <si>
+    <t>/decks/:deckId/flashcards/:flashcardId</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Auth &amp; ownership - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>certaines flashcards n'ont pas d'ID 1 sur un deck</t>
+    </r>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>list_public</t>
+  </si>
+  <si>
+    <t>list_owned</t>
+  </si>
+  <si>
+    <t>No Auth</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>publish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,13 +319,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -304,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,6 +370,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,21 +708,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADC9317-4E1B-4E09-9554-13BC2DDA84E4}">
-  <dimension ref="B2:E40"/>
+  <dimension ref="B2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
+    <col min="4" max="4" width="51.7265625" customWidth="1"/>
+    <col min="5" max="5" width="54.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="31.5">
+    <row r="2" spans="2:5" ht="31">
       <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
@@ -838,12 +893,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="31.5">
+    <row r="16" spans="2:5" ht="31">
       <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
@@ -856,9 +911,15 @@
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="2" t="s">
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -870,9 +931,12 @@
       <c r="E18" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="2" t="s">
+      <c r="F18" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -884,8 +948,11 @@
       <c r="E19" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="F19" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
@@ -898,8 +965,11 @@
       <c r="E20" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="F20" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
@@ -912,8 +982,11 @@
       <c r="E21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="F21" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
@@ -926,8 +999,11 @@
       <c r="E22" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="F22" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
       <c r="B23" s="2" t="s">
         <v>1</v>
       </c>
@@ -940,8 +1016,11 @@
       <c r="E23" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="F23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
@@ -954,13 +1033,16 @@
       <c r="E24" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" ht="31.5">
+      <c r="F24" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="31">
       <c r="B26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
@@ -973,50 +1055,65 @@
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="2" t="s">
+      <c r="F27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="29">
+      <c r="B28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="2:5">
+      <c r="F29" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="2:5">
+      <c r="F30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31" s="2" t="s">
         <v>3</v>
       </c>
@@ -1024,13 +1121,16 @@
         <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="2:5">
+      <c r="F31" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1038,15 +1138,18 @@
         <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" ht="31.5">
+      <c r="F32" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="31">
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="2:5">
@@ -1068,13 +1171,13 @@
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1082,13 +1185,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="2:5">
@@ -1096,13 +1199,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -1110,13 +1213,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>